<commit_message>
added simple bondPrice, NOT COMPLETE
</commit_message>
<xml_diff>
--- a/hw2/Bond.xlsx
+++ b/hw2/Bond.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5DBE3C5-33C6-492A-83B3-88B8D1A7BB85}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D0B261-87C1-4623-9227-190C7F3BA86A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="277" yWindow="473" windowWidth="20153" windowHeight="12277" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bond_example" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -144,9 +149,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -184,9 +189,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -219,26 +224,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -271,26 +259,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -464,18 +435,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:L14"/>
+  <dimension ref="A3:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -486,7 +458,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -497,7 +469,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -511,7 +483,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -525,7 +497,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -560,7 +532,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -568,11 +540,11 @@
         <v>11</v>
       </c>
       <c r="C9">
+        <f>100*$C$5*$C$4</f>
+        <v>4</v>
+      </c>
+      <c r="D9">
         <f t="shared" ref="C9:I9" si="0">100*$C$5*$C$4</f>
-        <v>4</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="E9">
@@ -603,7 +575,7 @@
         <v>101.6</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -647,7 +619,7 @@
         <v>0.74527649144328856</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -691,13 +663,165 @@
         <v>75.720091530638115</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K14" s="2">
         <f>SUM($C$12:K12)</f>
         <v>103.14493769298041</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>3</v>
+      </c>
+      <c r="F16">
+        <v>4</v>
+      </c>
+      <c r="G16">
+        <v>5</v>
+      </c>
+      <c r="H16">
+        <v>6</v>
+      </c>
+      <c r="I16">
+        <v>7</v>
+      </c>
+      <c r="J16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <f>100*$C$5*$C$4</f>
+        <v>4</v>
+      </c>
+      <c r="D17">
+        <f t="shared" ref="D17:J17" si="3">100*$C$5*$C$4</f>
+        <v>4</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="J17">
+        <f>4</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C18" s="1">
+        <f t="shared" ref="C18:J18" si="4">EXP(-$C$6*C16*$C$4)</f>
+        <v>0.96560541625756646</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" si="4"/>
+        <v>0.93239381990594827</v>
+      </c>
+      <c r="E18" s="1">
+        <f t="shared" si="4"/>
+        <v>0.90032452258626561</v>
+      </c>
+      <c r="F18" s="1">
+        <f t="shared" si="4"/>
+        <v>0.86935823539880586</v>
+      </c>
+      <c r="G18" s="1">
+        <f t="shared" si="4"/>
+        <v>0.83945702076920736</v>
+      </c>
+      <c r="H18" s="1">
+        <f t="shared" si="4"/>
+        <v>0.81058424597018708</v>
+      </c>
+      <c r="I18" s="1">
+        <f t="shared" si="4"/>
+        <v>0.78270453824186814</v>
+      </c>
+      <c r="J18" s="1">
+        <f t="shared" si="4"/>
+        <v>0.75578374145572547</v>
+      </c>
+    </row>
+    <row r="20" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <f>C17*C18</f>
+        <v>3.8624216650302658</v>
+      </c>
+      <c r="D20">
+        <f t="shared" ref="D20:J20" si="5">D17*D18</f>
+        <v>3.7295752796237931</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="5"/>
+        <v>3.6012980903450624</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="5"/>
+        <v>3.4774329415952234</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="5"/>
+        <v>3.3578280830768295</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="5"/>
+        <v>3.2423369838807483</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="5"/>
+        <v>3.1308181529674726</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="5"/>
+        <v>3.0231349658229019</v>
+      </c>
+    </row>
+    <row r="22" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <f>SUM(C20:F20)</f>
+        <v>14.670727976594344</v>
+      </c>
+      <c r="G22">
+        <f>SUM(C20:G20)</f>
+        <v>18.028556059671175</v>
+      </c>
+      <c r="H22">
+        <f>SUM(C20:H20)</f>
+        <v>21.270893043551922</v>
+      </c>
+      <c r="J22">
+        <f>SUM(C20:J20)</f>
+        <v>27.424846162342295</v>
+      </c>
+    </row>
+    <row r="25" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <f>100*0.08*0.5</f>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bondPrice function work with simple maturity timeframe
</commit_message>
<xml_diff>
--- a/hw2/Bond.xlsx
+++ b/hw2/Bond.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D0B261-87C1-4623-9227-190C7F3BA86A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55E806ED-568D-40A0-9B4A-50EADB92772B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -435,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:L25"/>
+  <dimension ref="A3:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,7 +544,7 @@
         <v>4</v>
       </c>
       <c r="D9">
-        <f t="shared" ref="C9:I9" si="0">100*$C$5*$C$4</f>
+        <f t="shared" ref="D9:I9" si="0">100*$C$5*$C$4</f>
         <v>4</v>
       </c>
       <c r="E9">
@@ -704,7 +704,7 @@
         <v>4</v>
       </c>
       <c r="D17">
-        <f t="shared" ref="D17:J17" si="3">100*$C$5*$C$4</f>
+        <f t="shared" ref="D17:I17" si="3">100*$C$5*$C$4</f>
         <v>4</v>
       </c>
       <c r="E17">
@@ -728,8 +728,7 @@
         <v>4</v>
       </c>
       <c r="J17">
-        <f>4</f>
-        <v>4</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="3:10" x14ac:dyDescent="0.25">
@@ -797,7 +796,7 @@
       </c>
       <c r="J20">
         <f t="shared" si="5"/>
-        <v>3.0231349658229019</v>
+        <v>78.601509111395444</v>
       </c>
     </row>
     <row r="22" spans="3:10" x14ac:dyDescent="0.25">
@@ -813,15 +812,13 @@
         <f>SUM(C20:H20)</f>
         <v>21.270893043551922</v>
       </c>
+      <c r="I22">
+        <f>SUM(C20:I20)</f>
+        <v>24.401711196519393</v>
+      </c>
       <c r="J22">
         <f>SUM(C20:J20)</f>
-        <v>27.424846162342295</v>
-      </c>
-    </row>
-    <row r="25" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C25">
-        <f>100*0.08*0.5</f>
-        <v>4</v>
+        <v>103.00322030791483</v>
       </c>
     </row>
   </sheetData>

</xml_diff>